<commit_message>
Casos de Testes executados e atualizados
</commit_message>
<xml_diff>
--- a/casos de testes/Casos de Testes - School Drive.xlsx
+++ b/casos de testes/Casos de Testes - School Drive.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="724" activeTab="3"/>
+    <workbookView xWindow="4020" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="724" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
   <si>
     <t>CAMPO</t>
   </si>
@@ -201,16 +201,7 @@
     </r>
   </si>
   <si>
-    <t>Cadastrar um novo Semestre com sucesso</t>
-  </si>
-  <si>
     <t>Cadastrar um novo semestre com um semestre aberto</t>
-  </si>
-  <si>
-    <t>Cadastrar um novo semestre com o ano do semestre menor ou igual ao anterior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadastrar um novo semestre com o ano maior que o ano atual </t>
   </si>
   <si>
     <t>2014.2</t>
@@ -247,193 +238,6 @@
         <family val="2"/>
       </rPr>
       <t>Abrir Novo Semestre</t>
-    </r>
-  </si>
-  <si>
-    <t>Sistema exibirá ao usuário a mensagem: "Não é possível criar um novo semestre com um semestre aberto"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ano e Semestre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> com os valores menores ou iguais aos últimos listados e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Abrir Novo Semestre</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ano e Semestre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> com dados válidos, ou não preencher e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Abrir Novo Semestre</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema exibirá a mensagem: "Não é possível criar um semestre com ano e semestre menor ou igual aos últimos listados"</t>
-  </si>
-  <si>
-    <r>
-      <t>Preencher o campo</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Ano e Semestre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> com o ano maior que o atual e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Abrir Novo Semestre</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema exibirá a mensagem: "Data de abertura do Semestre diferente do ano Atual"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cadastrar um novo semestre sem preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ano e Semestre</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Abrir Novo semestre </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">sem preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ano e Semestre</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema exibirá a mensagem: "Ano e semestres não informados"</t>
-  </si>
-  <si>
-    <t>2015.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2012.1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> | </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2014.2</t>
     </r>
   </si>
   <si>
@@ -691,10 +495,162 @@
     <t>Escolher Disciplina</t>
   </si>
   <si>
-    <t>Professor A</t>
+    <r>
+      <t xml:space="preserve">Preencher um semestre inválido (Ex.: 2014.5) no campo Ano e Semestre e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Abrir Novo semestre </t>
+    </r>
   </si>
   <si>
-    <t>Projeto de SW 2</t>
+    <t>O sistema exibirá a mensagem: "Semestre inválido!"</t>
+  </si>
+  <si>
+    <t>2014.3</t>
+  </si>
+  <si>
+    <t>Abrir um novo Semestre com sucesso</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Preencher o campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ano e Semestre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> com dados válidos, tendo um semestre aberto, e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Abrir Novo Semestre</t>
+    </r>
+  </si>
+  <si>
+    <t>Sistema exibirá ao usuário a mensagem: "Não é possível criar um novo semestre com um semestre aberto!!"</t>
+  </si>
+  <si>
+    <t>FALHOU! [Mensagem de retorno diferente da esperada]</t>
+  </si>
+  <si>
+    <t>PASSOU</t>
+  </si>
+  <si>
+    <t>2012.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastrar um novo semestre com o semestre menor ou igual ao último aberto </t>
+  </si>
+  <si>
+    <r>
+      <t>Preencher o campo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Ano e Semestre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> com o semestre menor/igual que o atual e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Abrir Novo Semestre</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema exibirá a mensagem: "Não é possível criar um semestre com o ano e ou Periodo, menor ou igual aos últimos listados!!"</t>
+  </si>
+  <si>
+    <t>2014.1</t>
+  </si>
+  <si>
+    <t>Cadastrar um novo semestre com o ano do semestre menor ou maior que o ano atual</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Preencher o campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ano e Semestre</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> com o ano menor/maior que o ano atual e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Abrir Novo Semestre</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema exibirá a mensagem: "Data de abertura do Semestre diferente do ano Atual !!"</t>
+  </si>
+  <si>
+    <t>Cadastrar um novo semestre inválido</t>
+  </si>
+  <si>
+    <t>FALHOU [Semestre inválido cadastrado]</t>
+  </si>
+  <si>
+    <t>Jarley Nobrega</t>
+  </si>
+  <si>
+    <t>Projeto de SW 1</t>
   </si>
 </sst>
 </file>
@@ -704,7 +660,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CT&quot;000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -792,6 +748,35 @@
       <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1161,7 +1146,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1348,20 +1333,23 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1369,11 +1357,14 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1396,32 +1387,59 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1834,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2231,10 +2249,10 @@
   <dimension ref="A1:IJ27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23:B24"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23:O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2250,43 +2268,45 @@
     <col min="9" max="9" width="5.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" style="21" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="21" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="21"/>
+    <col min="12" max="12" width="6.140625" style="21" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="21" customWidth="1"/>
-    <col min="16" max="17" width="5.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="21"/>
+    <col min="14" max="14" width="7.42578125" style="21" customWidth="1"/>
+    <col min="15" max="15" width="84.7109375" style="21" customWidth="1"/>
+    <col min="16" max="16" width="18" style="21" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="21" customWidth="1"/>
+    <col min="18" max="19" width="8.85546875" style="21" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:244" s="52" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
       <c r="S1" s="28"/>
       <c r="T1" s="38"/>
       <c r="U1" s="38"/>
@@ -2518,31 +2538,31 @@
       <c r="A2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="98" t="s">
-        <v>58</v>
+      <c r="B2" s="86" t="s">
+        <v>44</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="90" t="s">
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="90" t="s">
-        <v>36</v>
+      <c r="H2" s="92" t="s">
+        <v>33</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
       <c r="S2" s="28"/>
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
@@ -2774,25 +2794,25 @@
       <c r="A3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="28"/>
       <c r="T3" s="38"/>
       <c r="U3" s="38"/>
@@ -3021,28 +3041,28 @@
       <c r="IJ3" s="38"/>
     </row>
     <row r="4" spans="1:244" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="28"/>
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
@@ -3271,24 +3291,24 @@
       <c r="IJ4" s="38"/>
     </row>
     <row r="5" spans="1:244" x14ac:dyDescent="0.2">
-      <c r="A5" s="99"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="28"/>
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
@@ -4577,36 +4597,38 @@
       <c r="S11" s="22"/>
     </row>
     <row r="12" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
-        <v>51</v>
+      <c r="A12" s="79" t="s">
+        <v>37</v>
       </c>
-      <c r="B12" s="95" t="s">
-        <v>31</v>
+      <c r="B12" s="78" t="s">
+        <v>70</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="95" t="s">
-        <v>37</v>
+      <c r="D12" s="78" t="s">
+        <v>34</v>
       </c>
-      <c r="E12" s="83" t="s">
-        <v>50</v>
+      <c r="E12" s="84" t="s">
+        <v>36</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="86" t="s">
-        <v>35</v>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="98" t="s">
+        <v>32</v>
       </c>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
       <c r="S12" s="28"/>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -4835,24 +4857,24 @@
       <c r="IJ12" s="27"/>
     </row>
     <row r="13" spans="1:244" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
       <c r="S13" s="28"/>
       <c r="T13" s="27"/>
       <c r="U13" s="27"/>
@@ -5102,36 +5124,40 @@
       <c r="S14" s="22"/>
     </row>
     <row r="15" spans="1:244" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="101" t="s">
-        <v>52</v>
+      <c r="A15" s="79" t="s">
+        <v>38</v>
       </c>
-      <c r="B15" s="95" t="s">
-        <v>32</v>
+      <c r="B15" s="78" t="s">
+        <v>31</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="95" t="s">
-        <v>40</v>
+      <c r="D15" s="78" t="s">
+        <v>71</v>
       </c>
-      <c r="E15" s="85" t="s">
-        <v>38</v>
+      <c r="E15" s="99" t="s">
+        <v>72</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78" t="s">
-        <v>49</v>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96" t="s">
+        <v>35</v>
       </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="108" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
       <c r="S15" s="28"/>
       <c r="T15" s="27"/>
       <c r="U15" s="27"/>
@@ -5360,24 +5386,24 @@
       <c r="IJ15" s="27"/>
     </row>
     <row r="16" spans="1:244" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="102"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="97"/>
+      <c r="O16" s="109"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="97"/>
       <c r="S16" s="28"/>
       <c r="T16" s="27"/>
       <c r="U16" s="27"/>
@@ -5627,36 +5653,38 @@
       <c r="S17" s="22"/>
     </row>
     <row r="18" spans="1:244" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94" t="s">
-        <v>53</v>
+      <c r="A18" s="81" t="s">
+        <v>39</v>
       </c>
-      <c r="B18" s="83" t="s">
-        <v>33</v>
+      <c r="B18" s="84" t="s">
+        <v>80</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="83" t="s">
-        <v>39</v>
+      <c r="D18" s="84" t="s">
+        <v>81</v>
       </c>
-      <c r="E18" s="83" t="s">
-        <v>41</v>
+      <c r="E18" s="84" t="s">
+        <v>82</v>
       </c>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="82" t="s">
-        <v>48</v>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="110" t="s">
+        <v>75</v>
       </c>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="111" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="100"/>
+      <c r="R18" s="100"/>
       <c r="S18" s="28"/>
       <c r="T18" s="27"/>
       <c r="U18" s="27"/>
@@ -5885,24 +5913,24 @@
       <c r="IJ18" s="27"/>
     </row>
     <row r="19" spans="1:244" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+      <c r="N19" s="101"/>
+      <c r="O19" s="112"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+      <c r="R19" s="101"/>
       <c r="S19" s="28"/>
       <c r="T19" s="27"/>
       <c r="U19" s="27"/>
@@ -6153,24 +6181,24 @@
     </row>
     <row r="21" spans="1:244" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="73" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C21" s="58" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="59"/>
       <c r="H21" s="75" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="I21" s="60"/>
       <c r="J21" s="60"/>
@@ -6178,7 +6206,9 @@
       <c r="L21" s="61"/>
       <c r="M21" s="62"/>
       <c r="N21" s="62"/>
-      <c r="O21" s="62"/>
+      <c r="O21" s="113" t="s">
+        <v>74</v>
+      </c>
       <c r="P21" s="62"/>
       <c r="Q21" s="62"/>
       <c r="R21" s="62"/>
@@ -6431,35 +6461,41 @@
       <c r="S22" s="22"/>
     </row>
     <row r="23" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="94" t="s">
-        <v>55</v>
+      <c r="A23" s="81" t="s">
+        <v>41</v>
       </c>
-      <c r="B23" s="95" t="s">
-        <v>44</v>
+      <c r="B23" s="78" t="s">
+        <v>83</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="85" t="s">
-        <v>45</v>
+      <c r="D23" s="99" t="s">
+        <v>67</v>
       </c>
-      <c r="E23" s="85" t="s">
-        <v>46</v>
+      <c r="E23" s="99" t="s">
+        <v>68</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="P23" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
@@ -6687,25 +6723,25 @@
       <c r="IJ23" s="27"/>
     </row>
     <row r="24" spans="1:244" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="109"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="97"/>
+      <c r="S24" s="97"/>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -7222,12 +7258,78 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="R23:R24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:L5"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="Q2:Q5"/>
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="P2:P5"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
@@ -7244,78 +7346,12 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:L5"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="Q2:Q5"/>
-    <mergeCell ref="R2:R5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="R23:R24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:R10 H10">
     <cfRule type="cellIs" priority="15" operator="equal">
@@ -7356,11 +7392,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IJ27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:H5"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7388,31 +7424,31 @@
       <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
       <c r="S1" s="28"/>
       <c r="T1" s="38"/>
       <c r="U1" s="38"/>
@@ -7644,29 +7680,29 @@
       <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="98" t="s">
-        <v>58</v>
+      <c r="B2" s="86" t="s">
+        <v>44</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="90" t="s">
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
       <c r="S2" s="28"/>
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
@@ -7898,25 +7934,25 @@
       <c r="A3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="28"/>
       <c r="T3" s="38"/>
       <c r="U3" s="38"/>
@@ -8145,28 +8181,28 @@
       <c r="IJ3" s="38"/>
     </row>
     <row r="4" spans="1:244" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
-        <v>57</v>
+      <c r="B4" s="86" t="s">
+        <v>43</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="28"/>
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
@@ -8395,24 +8431,24 @@
       <c r="IJ4" s="38"/>
     </row>
     <row r="5" spans="1:244" x14ac:dyDescent="0.2">
-      <c r="A5" s="99"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="28"/>
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
@@ -9701,34 +9737,36 @@
       <c r="S11" s="22"/>
     </row>
     <row r="12" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
-        <v>51</v>
+      <c r="A12" s="79" t="s">
+        <v>37</v>
       </c>
-      <c r="B12" s="95" t="s">
-        <v>56</v>
+      <c r="B12" s="78" t="s">
+        <v>42</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="95" t="s">
-        <v>59</v>
+      <c r="D12" s="78" t="s">
+        <v>45</v>
       </c>
-      <c r="E12" s="83" t="s">
-        <v>61</v>
+      <c r="E12" s="84" t="s">
+        <v>47</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
       <c r="S12" s="28"/>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -9957,24 +9995,24 @@
       <c r="IJ12" s="27"/>
     </row>
     <row r="13" spans="1:244" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
       <c r="S13" s="28"/>
       <c r="T13" s="27"/>
       <c r="U13" s="27"/>
@@ -10224,32 +10262,34 @@
       <c r="S14" s="22"/>
     </row>
     <row r="15" spans="1:244" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="101"/>
-      <c r="B15" s="95" t="s">
-        <v>62</v>
+      <c r="A15" s="79"/>
+      <c r="B15" s="78" t="s">
+        <v>48</v>
       </c>
-      <c r="C15" s="95" t="s">
-        <v>60</v>
+      <c r="C15" s="78" t="s">
+        <v>46</v>
       </c>
-      <c r="D15" s="95" t="s">
-        <v>63</v>
+      <c r="D15" s="78" t="s">
+        <v>49</v>
       </c>
-      <c r="E15" s="85" t="s">
-        <v>64</v>
+      <c r="E15" s="99" t="s">
+        <v>50</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
       <c r="S15" s="28"/>
       <c r="T15" s="27"/>
       <c r="U15" s="27"/>
@@ -10478,24 +10518,24 @@
       <c r="IJ15" s="27"/>
     </row>
     <row r="16" spans="1:244" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="102"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="97"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="97"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="97"/>
       <c r="S16" s="28"/>
       <c r="T16" s="27"/>
       <c r="U16" s="27"/>
@@ -10745,24 +10785,24 @@
       <c r="S17" s="22"/>
     </row>
     <row r="18" spans="1:244" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="100"/>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="100"/>
+      <c r="R18" s="100"/>
       <c r="S18" s="28"/>
       <c r="T18" s="27"/>
       <c r="U18" s="27"/>
@@ -10991,24 +11031,24 @@
       <c r="IJ18" s="27"/>
     </row>
     <row r="19" spans="1:244" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+      <c r="N19" s="101"/>
+      <c r="O19" s="101"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+      <c r="R19" s="101"/>
       <c r="S19" s="28"/>
       <c r="T19" s="27"/>
       <c r="U19" s="27"/>
@@ -11525,25 +11565,25 @@
       <c r="S22" s="22"/>
     </row>
     <row r="23" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="94"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
@@ -11771,25 +11811,25 @@
       <c r="IJ23" s="27"/>
     </row>
     <row r="24" spans="1:244" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="97"/>
+      <c r="P24" s="97"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="97"/>
+      <c r="S24" s="97"/>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -12306,17 +12346,73 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E5"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:L5"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="R23:R24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="Q2:Q5"/>
     <mergeCell ref="R2:R5"/>
@@ -12333,73 +12429,17 @@
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="N2:N5"/>
     <mergeCell ref="O2:O5"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="R23:R24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E5"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:L5"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:R10 H10">
     <cfRule type="cellIs" priority="5" operator="equal">
@@ -12440,11 +12480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:I5"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12456,8 +12496,8 @@
     <col min="5" max="5" width="36.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="21" customWidth="1"/>
-    <col min="9" max="9" width="15" style="21" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="21" customWidth="1"/>
     <col min="10" max="10" width="11.140625" style="21" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="21" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="21"/>
@@ -12472,31 +12512,31 @@
       <c r="A1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
       <c r="S1" s="28"/>
       <c r="T1" s="38"/>
       <c r="U1" s="38"/>
@@ -12728,33 +12768,33 @@
       <c r="A2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="90" t="s">
-        <v>22</v>
+      <c r="I2" s="92" t="s">
+        <v>66</v>
       </c>
-      <c r="G2" s="90" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="90" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="90" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
       <c r="S2" s="28"/>
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
@@ -12986,25 +13026,25 @@
       <c r="A3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
       <c r="S3" s="28"/>
       <c r="T3" s="38"/>
       <c r="U3" s="38"/>
@@ -13233,28 +13273,28 @@
       <c r="IJ3" s="38"/>
     </row>
     <row r="4" spans="1:244" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="98" t="s">
-        <v>66</v>
+      <c r="B4" s="105" t="s">
+        <v>52</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
       <c r="S4" s="28"/>
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
@@ -13482,25 +13522,25 @@
       <c r="II4" s="38"/>
       <c r="IJ4" s="38"/>
     </row>
-    <row r="5" spans="1:244" x14ac:dyDescent="0.2">
-      <c r="A5" s="99"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
+    <row r="5" spans="1:244" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="87"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
       <c r="S5" s="28"/>
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
@@ -14516,16 +14556,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="67" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="32"/>
@@ -14789,38 +14829,40 @@
       <c r="S11" s="22"/>
     </row>
     <row r="12" spans="1:244" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
-        <v>51</v>
+      <c r="A12" s="79" t="s">
+        <v>37</v>
       </c>
-      <c r="B12" s="95" t="s">
-        <v>70</v>
+      <c r="B12" s="78" t="s">
+        <v>56</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="95" t="s">
-        <v>71</v>
+      <c r="D12" s="78" t="s">
+        <v>57</v>
       </c>
-      <c r="E12" s="83" t="s">
-        <v>72</v>
+      <c r="E12" s="84" t="s">
+        <v>58</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="86" t="s">
-        <v>81</v>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="98" t="s">
+        <v>85</v>
       </c>
-      <c r="I12" s="86" t="s">
-        <v>82</v>
+      <c r="I12" s="98" t="s">
+        <v>86</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
       <c r="S12" s="28"/>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -15049,24 +15091,24 @@
       <c r="IJ12" s="27"/>
     </row>
     <row r="13" spans="1:244" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
       <c r="S13" s="28"/>
       <c r="T13" s="27"/>
       <c r="U13" s="27"/>
@@ -15316,34 +15358,36 @@
       <c r="S14" s="22"/>
     </row>
     <row r="15" spans="1:244" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="101" t="s">
-        <v>52</v>
+      <c r="A15" s="79" t="s">
+        <v>38</v>
       </c>
-      <c r="B15" s="95" t="s">
-        <v>73</v>
+      <c r="B15" s="78" t="s">
+        <v>59</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="95" t="s">
-        <v>75</v>
+      <c r="D15" s="78" t="s">
+        <v>61</v>
       </c>
-      <c r="E15" s="85" t="s">
-        <v>76</v>
+      <c r="E15" s="99" t="s">
+        <v>62</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
       <c r="S15" s="28"/>
       <c r="T15" s="27"/>
       <c r="U15" s="27"/>
@@ -15572,24 +15616,24 @@
       <c r="IJ15" s="27"/>
     </row>
     <row r="16" spans="1:244" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="102"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="97"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="97"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="97"/>
       <c r="S16" s="28"/>
       <c r="T16" s="27"/>
       <c r="U16" s="27"/>
@@ -15839,34 +15883,36 @@
       <c r="S17" s="22"/>
     </row>
     <row r="18" spans="1:244" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94" t="s">
-        <v>53</v>
+      <c r="A18" s="81" t="s">
+        <v>39</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="95" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="83" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="100"/>
+      <c r="R18" s="100"/>
       <c r="S18" s="28"/>
       <c r="T18" s="27"/>
       <c r="U18" s="27"/>
@@ -16095,24 +16141,24 @@
       <c r="IJ18" s="27"/>
     </row>
     <row r="19" spans="1:244" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+      <c r="N19" s="101"/>
+      <c r="O19" s="112"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+      <c r="R19" s="101"/>
       <c r="S19" s="28"/>
       <c r="T19" s="27"/>
       <c r="U19" s="27"/>
@@ -16629,25 +16675,25 @@
       <c r="S22" s="22"/>
     </row>
     <row r="23" spans="1:244" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="94"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
       <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
@@ -16875,25 +16921,25 @@
       <c r="IJ23" s="27"/>
     </row>
     <row r="24" spans="1:244" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="97"/>
+      <c r="P24" s="97"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="97"/>
+      <c r="S24" s="97"/>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -17410,17 +17456,73 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E5"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:L5"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="R23:R24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="Q2:Q5"/>
     <mergeCell ref="R2:R5"/>
@@ -17437,73 +17539,17 @@
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="N2:N5"/>
     <mergeCell ref="O2:O5"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="R23:R24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E5"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:L5"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:R10 H10">
     <cfRule type="cellIs" priority="5" operator="equal">

</xml_diff>